<commit_message>
Changed browser name in testng.xml
</commit_message>
<xml_diff>
--- a/src/test/java/com/practice/testData/UserData.xlsx
+++ b/src/test/java/com/practice/testData/UserData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14520" windowHeight="4590"/>
+    <workbookView windowWidth="23040" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="ValidData" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="InvalidData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:B1"/>
 </workbook>
 </file>
 
@@ -135,9 +134,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -157,13 +156,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -172,6 +164,30 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,48 +209,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,45 +240,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,13 +314,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,7 +434,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,25 +476,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -375,127 +494,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,17 +508,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,25 +557,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -589,6 +588,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -597,162 +605,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -763,7 +762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -778,12 +777,12 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
     <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
@@ -1094,10 +1093,10 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.73148148148148" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="30.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="20.0909090909091" customWidth="1"/>
+    <col min="1" max="1" width="30.2685185185185" customWidth="1"/>
+    <col min="2" max="2" width="20.0925925925926" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1248,7 +1247,7 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>1234567890</v>
+        <v>9898989989</v>
       </c>
     </row>
     <row r="22" spans="1:1">
@@ -1280,7 +1279,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.73148148148148" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1296,7 +1295,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.73148148148148" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>